<commit_message>
start working on loading network
</commit_message>
<xml_diff>
--- a/freezedried_data/dataToLoad.v3.xlsx
+++ b/freezedried_data/dataToLoad.v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Farmers" sheetId="1" state="visible" r:id="rId2"/>
@@ -309,7 +309,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -352,7 +352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -438,10 +438,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -459,23 +459,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixing exceldataloader for arablebehavior. crops finished
</commit_message>
<xml_diff>
--- a/freezedried_data/dataToLoad.v3.xlsx
+++ b/freezedried_data/dataToLoad.v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Farmers" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Agent_id</t>
   </si>
@@ -79,7 +79,7 @@
     <t>maize seeds</t>
   </si>
   <si>
-    <t>durum wheat</t>
+    <t>wheat</t>
   </si>
   <si>
     <t>durum wheat seeds</t>
@@ -95,12 +95,6 @@
   </si>
   <si>
     <t>animal food</t>
-  </si>
-  <si>
-    <t>tobbaco</t>
-  </si>
-  <si>
-    <t>tobbaco leaves</t>
   </si>
   <si>
     <t>plot_id</t>
@@ -440,8 +434,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3133,13 +3127,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.8622448979592"/>
@@ -3198,17 +3192,6 @@
       </c>
       <c r="D4" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -14770,13 +14753,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
finished excel loading for arablecropbehavior !
</commit_message>
<xml_diff>
--- a/freezedried_data/dataToLoad.v3.xlsx
+++ b/freezedried_data/dataToLoad.v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Farmers" sheetId="1" state="visible" r:id="rId2"/>
@@ -303,11 +303,11 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.70918367346939"/>
@@ -317,7 +317,8 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.5765306122449"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.7091836734694"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="1" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,7 +361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -374,7 +375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
@@ -388,7 +389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
@@ -402,7 +403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
@@ -3129,7 +3130,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Immitator-kind of arablecropproductionbehavior finished
</commit_message>
<xml_diff>
--- a/freezedried_data/dataToLoad.v3.xlsx
+++ b/freezedried_data/dataToLoad.v3.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Agent_id</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Farmer_MP</t>
+  </si>
+  <si>
+    <t>Farmer_Imm</t>
   </si>
   <si>
     <t>Farmer_Net</t>
@@ -304,7 +307,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -386,7 +389,7 @@
         <v>100000</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,7 +403,7 @@
         <v>100000</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,7 +417,7 @@
         <v>100000</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -448,10 +451,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,7 +502,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>0</v>
@@ -3145,13 +3148,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="0"/>
     </row>
@@ -3160,10 +3163,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0"/>
     </row>
@@ -3172,13 +3175,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,13 +3189,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3224,7 +3227,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>0</v>
@@ -6106,7 +6109,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>0</v>
@@ -8988,7 +8991,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>0</v>
@@ -11872,7 +11875,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="n">
         <v>1</v>
@@ -14754,13 +14757,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>